<commit_message>
add daily, weekly, monthly ntfy channels, automatic commit
</commit_message>
<xml_diff>
--- a/data/feature-extraction/transformersjs_08-05-2024.xlsx
+++ b/data/feature-extraction/transformersjs_08-05-2024.xlsx
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1619336</v>
+        <v>1755877</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>65733</v>
+        <v>75109</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>18453</v>
+        <v>19315</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -944,7 +944,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>31704</v>
+        <v>33257</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -1013,7 +1013,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7391</v>
+        <v>7756</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -1151,7 +1151,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>11377</v>
+        <v>10108</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1220,7 +1220,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>11864</v>
+        <v>10853</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>96117</v>
+        <v>97301</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1565,7 +1565,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>35020</v>
+        <v>35205</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -10259,7 +10259,7 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>7095</v>
+        <v>7547</v>
       </c>
       <c r="E143" t="b">
         <v>0</v>
@@ -10328,7 +10328,7 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>3149</v>
+        <v>3472</v>
       </c>
       <c r="E144" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Add generated model files
</commit_message>
<xml_diff>
--- a/data/feature-extraction/transformersjs_08-05-2024.xlsx
+++ b/data/feature-extraction/transformersjs_08-05-2024.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -728,36 +728,36 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Alibaba-NLP</t>
+          <t>WhereIsAI</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'avatarUrl': 'https://www.gravatar.com/avatar/1ae3fd9f5b9356f196c997d93eb23038?d=retro&amp;size=100', 'fullname': 'Alibaba-NLP', 'name': 'Alibaba-NLP', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
+          <t>{'avatarUrl': 'https://www.gravatar.com/avatar/e81bd32cb5ee88835824ad6b60d05697?d=retro&amp;size=100', 'fullname': 'WhereIsAI', 'name': 'WhereIsAI', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>75109</v>
+        <v>277613</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Alibaba-NLP/gte-large-en-v1.5</t>
+          <t>WhereIsAI/UAE-Large-V1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2024-04-26T13:51:26.000Z</t>
+          <t>2024-05-03T02:31:54.000Z</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>56</v>
+        <v>177</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>sentence-similarity</t>
+          <t>feature-extraction</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -773,14 +773,14 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>1.75GB | 361MB | 873MB | 446MB | 387MB | 446MB | 446MB</t>
+          <t>1.34GB | 669MB | 337MB</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>378535936</v>
+        <v>353370112</v>
       </c>
       <c r="O5" t="n">
-        <v>1879048192</v>
+        <v>1438814044.16</v>
       </c>
       <c r="P5" t="n">
         <v>4</v>
@@ -797,36 +797,36 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>WhereIsAI</t>
+          <t>Snowflake</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'avatarUrl': 'https://www.gravatar.com/avatar/e81bd32cb5ee88835824ad6b60d05697?d=retro&amp;size=100', 'fullname': 'WhereIsAI', 'name': 'WhereIsAI', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
+          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/64ba2f59a6ccf0f64b4ad254/eTDA37yFwUVP45c1WTSs2.png', 'fullname': 'Snowflake', 'name': 'Snowflake', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>277613</v>
+        <v>33257</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>WhereIsAI/UAE-Large-V1</t>
+          <t>Snowflake/snowflake-arctic-embed-l</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2024-05-03T02:31:54.000Z</t>
+          <t>2024-04-18T19:58:11.000Z</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>177</v>
+        <v>58</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>feature-extraction</t>
+          <t>sentence-similarity</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -842,11 +842,11 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>1.34GB | 669MB | 337MB</t>
+          <t>1.34GB | 299MB | 669MB | 337MB | 318MB | 337MB | 337MB</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>353370112</v>
+        <v>313524224</v>
       </c>
       <c r="O6" t="n">
         <v>1438814044.16</v>
@@ -935,32 +935,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Snowflake</t>
+          <t>Alibaba-NLP</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/64ba2f59a6ccf0f64b4ad254/eTDA37yFwUVP45c1WTSs2.png', 'fullname': 'Snowflake', 'name': 'Snowflake', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
+          <t>{'avatarUrl': 'https://www.gravatar.com/avatar/1ae3fd9f5b9356f196c997d93eb23038?d=retro&amp;size=100', 'fullname': 'Alibaba-NLP', 'name': 'Alibaba-NLP', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>33257</v>
+        <v>75109</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Snowflake/snowflake-arctic-embed-l</t>
+          <t>Alibaba-NLP/gte-large-en-v1.5</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2024-04-18T19:58:11.000Z</t>
+          <t>2024-04-26T13:51:26.000Z</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -980,14 +980,14 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>1.34GB | 299MB | 669MB | 337MB | 318MB | 337MB | 337MB</t>
+          <t>1.75GB | 361MB | 873MB | 446MB | 387MB | 446MB | 446MB</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>313524224</v>
+        <v>378535936</v>
       </c>
       <c r="O8" t="n">
-        <v>1438814044.16</v>
+        <v>1879048192</v>
       </c>
       <c r="P8" t="n">
         <v>7</v>
@@ -1280,36 +1280,36 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Alibaba-NLP</t>
+          <t>Xenova</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'avatarUrl': 'https://www.gravatar.com/avatar/1ae3fd9f5b9356f196c997d93eb23038?d=retro&amp;size=100', 'fullname': 'Alibaba-NLP', 'name': 'Alibaba-NLP', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
+          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/61b253b7ac5ecaae3d1efe0c/hwiQ0uvz3t-L5a-NtBIO6.png', 'fullname': 'Joshua', 'name': 'Xenova', 'type': 'user', 'isPro': False, 'isHf': True}</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>97301</v>
+        <v>105</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Alibaba-NLP/gte-base-en-v1.5</t>
+          <t>Xenova/all-MiniLM-L6-v2</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2024-04-26T13:53:41.000Z</t>
+          <t>2024-03-12T03:11:08.000Z</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>sentence-similarity</t>
+          <t>feature-extraction</t>
         </is>
       </c>
       <c r="J13" t="b">
@@ -1325,14 +1325,14 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>556MB | 167MB | 278MB | 147MB | 174MB | 147MB | 147MB</t>
+          <t>90.4MB | 45.3MB | 23MB | 23MB</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>154140672</v>
+        <v>24117248</v>
       </c>
       <c r="O13" t="n">
-        <v>583008256</v>
+        <v>94791270.40000001</v>
       </c>
       <c r="P13" t="n">
         <v>12</v>
@@ -1358,23 +1358,23 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>105</v>
+        <v>3</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Xenova/all-MiniLM-L6-v2</t>
+          <t>Xenova/larger_clap_music_and_speech</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2024-03-12T03:11:08.000Z</t>
+          <t>2024-03-17T15:10:25.000Z</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1394,14 +1394,14 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>90.4MB | 45.3MB | 23MB | 23MB</t>
+          <t>783MB | 395MB | 205MB</t>
         </is>
       </c>
       <c r="N14" t="n">
-        <v>24117248</v>
+        <v>214958080</v>
       </c>
       <c r="O14" t="n">
-        <v>94791270.40000001</v>
+        <v>821035008</v>
       </c>
       <c r="P14" t="n">
         <v>13</v>
@@ -1418,32 +1418,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Xenova</t>
+          <t>jinaai</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/61b253b7ac5ecaae3d1efe0c/hwiQ0uvz3t-L5a-NtBIO6.png', 'fullname': 'Joshua', 'name': 'Xenova', 'type': 'user', 'isPro': False, 'isHf': True}</t>
+          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/603763514de52ff951d89793/AFoybzd5lpBQXEBrQHuTt.png', 'fullname': 'Jina AI', 'name': 'jinaai', 'type': 'org', 'isHf': False, 'isEnterprise': True}</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>20417</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Xenova/larger_clap_music_and_speech</t>
+          <t>jinaai/jina-embeddings-v2-base-de</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2024-03-17T15:10:25.000Z</t>
+          <t>2024-04-26T07:35:44.000Z</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1463,14 +1463,14 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>783MB | 395MB | 205MB</t>
+          <t>641MB | 321MB | 162MB</t>
         </is>
       </c>
       <c r="N15" t="n">
-        <v>214958080</v>
+        <v>169869312</v>
       </c>
       <c r="O15" t="n">
-        <v>821035008</v>
+        <v>672137216</v>
       </c>
       <c r="P15" t="n">
         <v>14</v>
@@ -1487,32 +1487,32 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>jinaai</t>
+          <t>mixedbread-ai</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/603763514de52ff951d89793/AFoybzd5lpBQXEBrQHuTt.png', 'fullname': 'Jina AI', 'name': 'jinaai', 'type': 'org', 'isHf': False, 'isEnterprise': True}</t>
+          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/643ee0870d1194da249bd7fe/voYdYlFgQH5vyMwyMNluZ.png', 'fullname': 'mixedbread ai', 'name': 'mixedbread-ai', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>20417</v>
+        <v>35205</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>jinaai/jina-embeddings-v2-base-de</t>
+          <t>mixedbread-ai/mxbai-embed-2d-large-v1</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2024-04-26T07:35:44.000Z</t>
+          <t>2024-04-04T21:36:56.000Z</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1532,14 +1532,14 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>641MB | 321MB | 162MB</t>
+          <t>1.34GB | 669MB | 337MB</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>169869312</v>
+        <v>353370112</v>
       </c>
       <c r="O16" t="n">
-        <v>672137216</v>
+        <v>1438814044.16</v>
       </c>
       <c r="P16" t="n">
         <v>15</v>
@@ -1556,32 +1556,32 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>mixedbread-ai</t>
+          <t>Xenova</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/643ee0870d1194da249bd7fe/voYdYlFgQH5vyMwyMNluZ.png', 'fullname': 'mixedbread ai', 'name': 'mixedbread-ai', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
+          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/61b253b7ac5ecaae3d1efe0c/hwiQ0uvz3t-L5a-NtBIO6.png', 'fullname': 'Joshua', 'name': 'Xenova', 'type': 'user', 'isPro': False, 'isHf': True}</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>35205</v>
+        <v>3</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>mixedbread-ai/mxbai-embed-2d-large-v1</t>
+          <t>Xenova/text2vec-base-chinese-paraphrase</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2024-04-04T21:36:56.000Z</t>
+          <t>2024-03-23T00:34:15.000Z</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1601,14 +1601,14 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>1.34GB | 669MB | 337MB</t>
+          <t>470MB | 178MB | 235MB | 119MB | 183MB | 119MB | 119MB</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>353370112</v>
+        <v>124780544</v>
       </c>
       <c r="O17" t="n">
-        <v>1438814044.16</v>
+        <v>492830720</v>
       </c>
       <c r="P17" t="n">
         <v>16</v>
@@ -1625,36 +1625,36 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Xenova</t>
+          <t>Alibaba-NLP</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'avatarUrl': 'https://cdn-avatars.huggingface.co/v1/production/uploads/61b253b7ac5ecaae3d1efe0c/hwiQ0uvz3t-L5a-NtBIO6.png', 'fullname': 'Joshua', 'name': 'Xenova', 'type': 'user', 'isPro': False, 'isHf': True}</t>
+          <t>{'avatarUrl': 'https://www.gravatar.com/avatar/1ae3fd9f5b9356f196c997d93eb23038?d=retro&amp;size=100', 'fullname': 'Alibaba-NLP', 'name': 'Alibaba-NLP', 'type': 'org', 'isHf': False, 'isEnterprise': False}</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>97301</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Xenova/text2vec-base-chinese-paraphrase</t>
+          <t>Alibaba-NLP/gte-base-en-v1.5</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2024-03-23T00:34:15.000Z</t>
+          <t>2024-04-26T13:53:41.000Z</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>feature-extraction</t>
+          <t>sentence-similarity</t>
         </is>
       </c>
       <c r="J18" t="b">
@@ -1670,14 +1670,14 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>470MB | 178MB | 235MB | 119MB | 183MB | 119MB | 119MB</t>
+          <t>556MB | 167MB | 278MB | 147MB | 174MB | 147MB | 147MB</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>124780544</v>
+        <v>154140672</v>
       </c>
       <c r="O18" t="n">
-        <v>492830720</v>
+        <v>583008256</v>
       </c>
       <c r="P18" t="n">
         <v>17</v>

</xml_diff>